<commit_message>
Added Pie Chart Function
</commit_message>
<xml_diff>
--- a/Water Footprint Calculator.xlsx
+++ b/Water Footprint Calculator.xlsx
@@ -105,17 +105,17 @@
     <t>Footprint (L)</t>
   </si>
   <si>
-    <t>Total Footprint</t>
-  </si>
-  <si>
     <t>Water Foot Print (L/Kg)</t>
+  </si>
+  <si>
+    <t>Total Water Footprint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,12 +142,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -212,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,14 +218,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,6 +235,309 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="134"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="34"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Water Footprint</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="75"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>Oil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bread(from Wheat)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Potatoes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Butter</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Noodles</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Water</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cheese</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Red Chilli Powder</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Rice</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Chicken</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Onion</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Ground Nuts</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Flour</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Vinegar</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Pepper</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Garlic</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Curd</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Carrots</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Eggs</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Peas</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Soy Sauce</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Cabbage</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Coriander Powder</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Pork</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Sugar</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Chocolate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,59 +830,66 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>3400</v>
+        <v>4971</v>
       </c>
       <c r="D2" s="3">
         <f>B2*C2</f>
         <v>0</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="7">
+        <f>SUM(D2:D27)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>1849</v>
+        <v>1300</v>
       </c>
       <c r="D3" s="4">
         <f>B3*C3</f>
@@ -597,13 +898,13 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>5533</v>
+        <v>250</v>
       </c>
       <c r="D4" s="4">
         <f>B4*C4</f>
@@ -612,13 +913,13 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>250</v>
+        <v>5533</v>
       </c>
       <c r="D5" s="4">
         <f>B5*C5</f>
@@ -627,65 +928,59 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>7365</v>
-      </c>
-      <c r="D6" s="4">
+        <v>1673</v>
+      </c>
+      <c r="D6" s="3">
         <f>B6*C6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>39</v>
+        <f>B7</f>
+        <v>0</v>
       </c>
       <c r="D7" s="4">
-        <f>B7*C7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>13</v>
+        <f>C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>1600</v>
+        <v>5000</v>
       </c>
       <c r="D8" s="4">
         <f>B8*C8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="8">
-        <f>SUM(D2:D27)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4">
         <v>0</v>
       </c>
       <c r="C9" s="2">
-        <v>195</v>
+        <v>39</v>
       </c>
       <c r="D9" s="4">
         <f>B9*C9</f>
@@ -694,13 +989,13 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>3300</v>
+        <v>3400</v>
       </c>
       <c r="D10" s="3">
         <f>B10*C10</f>
@@ -709,44 +1004,43 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4">
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>4971</v>
-      </c>
-      <c r="D11" s="3">
+        <v>3900</v>
+      </c>
+      <c r="D11" s="4">
         <f>B11*C11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <f>B12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <f>C12</f>
+        <v>345</v>
+      </c>
+      <c r="D12" s="3">
+        <f>B12*C12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="3">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4">
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>589</v>
+        <v>3100</v>
       </c>
       <c r="D13" s="4">
         <f>B13*C13</f>
@@ -755,13 +1049,13 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>5000</v>
+        <v>1849</v>
       </c>
       <c r="D14" s="4">
         <f>B14*C14</f>
@@ -770,13 +1064,13 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>3900</v>
+        <v>1600</v>
       </c>
       <c r="D15" s="4">
         <f>B15*C15</f>
@@ -785,118 +1079,118 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
         <v>0</v>
       </c>
       <c r="C16" s="2">
-        <v>345</v>
-      </c>
-      <c r="D16" s="3">
+        <v>7365</v>
+      </c>
+      <c r="D16" s="4">
         <f>B16*C16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
       </c>
       <c r="C17" s="2">
-        <v>595</v>
-      </c>
-      <c r="D17" s="3">
+        <v>589</v>
+      </c>
+      <c r="D17" s="4">
         <f>B17*C17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="2">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4">
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <v>1673</v>
-      </c>
-      <c r="D18" s="3">
+        <v>600</v>
+      </c>
+      <c r="D18" s="4">
         <f>B18*C18</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>1035</v>
-      </c>
-      <c r="D19" s="3">
+        <v>195</v>
+      </c>
+      <c r="D19" s="4">
         <f>B19*C19</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3">
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <v>280</v>
-      </c>
-      <c r="D20" s="4">
+        <v>3300</v>
+      </c>
+      <c r="D20" s="3">
         <f>B20*C20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3">
         <v>0</v>
       </c>
       <c r="C21" s="2">
-        <v>8280</v>
-      </c>
-      <c r="D21" s="4">
+        <v>595</v>
+      </c>
+      <c r="D21" s="3">
         <f>B21*C21</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>4800</v>
-      </c>
-      <c r="D22" s="4">
+        <v>1035</v>
+      </c>
+      <c r="D22" s="3">
         <f>B22*C22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <v>1500</v>
+        <v>280</v>
       </c>
       <c r="D23" s="4">
         <f>B23*C23</f>
@@ -905,13 +1199,13 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B24" s="4">
         <v>0</v>
       </c>
       <c r="C24" s="2">
-        <v>1300</v>
+        <v>8280</v>
       </c>
       <c r="D24" s="4">
         <f>B24*C24</f>
@@ -920,13 +1214,13 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="4">
         <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>24000</v>
+        <v>4800</v>
       </c>
       <c r="D25" s="4">
         <f>B25*C25</f>
@@ -935,13 +1229,13 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4">
         <v>0</v>
       </c>
       <c r="C26" s="2">
-        <v>3100</v>
+        <v>1500</v>
       </c>
       <c r="D26" s="4">
         <f>B26*C26</f>
@@ -950,11 +1244,13 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0</v>
+      </c>
       <c r="C27" s="2">
-        <v>600</v>
+        <v>24000</v>
       </c>
       <c r="D27" s="4">
         <f>B27*C27</f>
@@ -966,6 +1262,7 @@
     <sortCondition descending="1" ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>